<commit_message>
chỉnh front end list-exam
</commit_message>
<xml_diff>
--- a/Testing_System/bin/files/exam.xlsx
+++ b/Testing_System/bin/files/exam.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
-  <si>
-    <t>examId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -30,100 +27,60 @@
     <t>note</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>isEnable</t>
-  </si>
-  <si>
     <t>numberOfQuestion</t>
   </si>
   <si>
-    <t>createAt</t>
-  </si>
-  <si>
-    <t>createBy</t>
-  </si>
-  <si>
-    <t>modifiedAt</t>
-  </si>
-  <si>
-    <t>modifiedBy</t>
-  </si>
-  <si>
-    <t>java123</t>
-  </si>
-  <si>
     <t>de01</t>
   </si>
   <si>
-    <t>java124</t>
-  </si>
-  <si>
     <t>de02</t>
   </si>
   <si>
     <t>asf</t>
   </si>
   <si>
-    <t>python01</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
-    <t>lvchai2</t>
-  </si>
-  <si>
     <t>bbh</t>
   </si>
   <si>
     <t>jvj</t>
   </si>
   <si>
-    <t>draft</t>
-  </si>
-  <si>
-    <t>public</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>fsdf</t>
-  </si>
-  <si>
-    <t>Angular02</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>2019-07-02</t>
-  </si>
-  <si>
-    <t>2019-02-02</t>
-  </si>
-  <si>
-    <t>2019-02-18</t>
-  </si>
-  <si>
-    <t>2019-02-19</t>
+    <t>categoryId</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>de03</t>
+  </si>
+  <si>
+    <t>C#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,12 +110,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -254,7 +211,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -431,7 +388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -439,197 +396,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="B2" s="4">
+        <v>90</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4">
+        <v>60</v>
+      </c>
+      <c r="F2"/>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B3" s="4">
+        <v>90</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="E3" s="4">
+        <v>60</v>
+      </c>
+      <c r="F3"/>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4">
+        <v>90</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="E4" s="4">
         <v>90</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="5">
-        <v>60</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5">
-        <v>90</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5">
-        <v>60</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5">
-        <v>90</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="5">
-        <v>90</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5">
-        <v>40</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="5">
-        <v>60</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="1"/>
+      <c r="F4"/>
+      <c r="H4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>